<commit_message>
update testcase name and add Allure report clean data code.
</commit_message>
<xml_diff>
--- a/TestData/PythonDemo.xlsx
+++ b/TestData/PythonDemo.xlsx
@@ -1017,14 +1017,14 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9.77777777777778" customWidth="1"/>
-    <col min="2" max="2" width="6.88888888888889" customWidth="1"/>
-    <col min="3" max="3" width="9.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="9.44444444444444" customWidth="1"/>
+    <col min="3" max="3" width="9.11111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>